<commit_message>
feat: started spreadsheet loading
</commit_message>
<xml_diff>
--- a/model/database.xlsx
+++ b/model/database.xlsx
@@ -17,12 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>codigo</t>
-  </si>
-  <si>
-    <t>nome</t>
   </si>
   <si>
     <t>manhã</t>
@@ -86,8 +83,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -115,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,95 +427,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -519,157 +544,174 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -685,6 +727,12 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -693,36 +741,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>2</v>
       </c>
     </row>

</xml_diff>